<commit_message>
fix material database filed line traces example
</commit_message>
<xml_diff>
--- a/pyaedt/field_line_traces/my_copper.xlsx
+++ b/pyaedt/field_line_traces/my_copper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbertonc\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnsysDev\NoBackup\example-data\pyaedt\field_line_traces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9936EC-026F-4F47-A84A-94A972B8EC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC66100E-B0FA-451D-8D1E-C86F35D80CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="6495" windowWidth="21600" windowHeight="12735" xr2:uid="{0C1F8FD3-C74D-460F-8E6A-2330938BCBF0}"/>
+    <workbookView xWindow="-23148" yWindow="4308" windowWidth="23256" windowHeight="12576" xr2:uid="{0C1F8FD3-C74D-460F-8E6A-2330938BCBF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,13 +41,13 @@
     <t>my_copper</t>
   </si>
   <si>
-    <t>material bulk conductivity</t>
+    <t>material name</t>
   </si>
   <si>
-    <t>material relative permittivity</t>
+    <t>Conductivity</t>
   </si>
   <si>
-    <t>material name</t>
+    <t>permittivity</t>
   </si>
 </sst>
 </file>
@@ -402,28 +402,28 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fix material database filed line traces example (#120)
</commit_message>
<xml_diff>
--- a/pyaedt/field_line_traces/my_copper.xlsx
+++ b/pyaedt/field_line_traces/my_copper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbertonc\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnsysDev\NoBackup\example-data\pyaedt\field_line_traces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9936EC-026F-4F47-A84A-94A972B8EC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC66100E-B0FA-451D-8D1E-C86F35D80CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="6495" windowWidth="21600" windowHeight="12735" xr2:uid="{0C1F8FD3-C74D-460F-8E6A-2330938BCBF0}"/>
+    <workbookView xWindow="-23148" yWindow="4308" windowWidth="23256" windowHeight="12576" xr2:uid="{0C1F8FD3-C74D-460F-8E6A-2330938BCBF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,13 +41,13 @@
     <t>my_copper</t>
   </si>
   <si>
-    <t>material bulk conductivity</t>
+    <t>material name</t>
   </si>
   <si>
-    <t>material relative permittivity</t>
+    <t>Conductivity</t>
   </si>
   <si>
-    <t>material name</t>
+    <t>permittivity</t>
   </si>
 </sst>
 </file>
@@ -402,28 +402,28 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>